<commit_message>
nysa date and vahan few lines fixed
</commit_message>
<xml_diff>
--- a/policy_details.xlsx
+++ b/policy_details.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -441,10 +441,10 @@
         <v>Pahadiya Commercial Ltd</v>
       </c>
       <c r="C2" t="str">
-        <v>3005/405543780/00/000</v>
+        <v>3005/406511857/00/000</v>
       </c>
       <c r="D2" t="str">
-        <v>ME4JC94CGSG140743</v>
+        <v>ME4JC94CGSG140727</v>
       </c>
       <c r="E2" t="str">
         <v>TWO WHEELER</v>
@@ -453,19 +453,19 @@
         <v>New Business</v>
       </c>
       <c r="G2" t="str">
-        <v>2025-08-27T16:59:34.435959</v>
+        <v>2025-08-31T12:37:13.827032</v>
       </c>
       <c r="H2" t="str">
-        <v>Satyendra Kumar</v>
+        <v>Arvind Kumar Prasad</v>
       </c>
       <c r="I2" t="str">
         <v>6103</v>
       </c>
       <c r="J2" t="str">
-        <v>1245192604</v>
+        <v>1245534626</v>
       </c>
       <c r="K2" t="str">
-        <v>855854</v>
+        <v>566988</v>
       </c>
       <c r="M2" t="str">
         <v>HONDA MOTORCYCLE</v>
@@ -491,10 +491,10 @@
         <v>Pahadiya Commercial Ltd</v>
       </c>
       <c r="C3" t="str">
-        <v>3005/O/405689325/00/B00</v>
+        <v>3005/O/405811018/00/000</v>
       </c>
       <c r="D3" t="str">
-        <v>ME1RG661BL0074373</v>
+        <v>ME4JK13BHPG003866</v>
       </c>
       <c r="E3" t="str">
         <v>TWO WHEELER</v>
@@ -503,25 +503,28 @@
         <v>Roll Over</v>
       </c>
       <c r="G3" t="str">
-        <v>2025-08-28T16:40:11.211006</v>
+        <v>2025-08-29T11:39:16.619518</v>
       </c>
       <c r="H3" t="str">
-        <v>Manish Kumar</v>
+        <v>Munna Kumar</v>
       </c>
       <c r="I3" t="str">
-        <v>1264</v>
+        <v>1611</v>
       </c>
       <c r="J3" t="str">
-        <v>12345678</v>
+        <v>1245389166</v>
+      </c>
+      <c r="K3" t="str">
+        <v>855484</v>
       </c>
       <c r="M3" t="str">
-        <v>YAMAHA</v>
+        <v>HONDA MOTORCYCLE</v>
       </c>
       <c r="N3" t="str">
-        <v>FZ S FI BT BS VI</v>
+        <v>ACTIVA 125 DRUM</v>
       </c>
       <c r="O3" t="str">
-        <v>Insta</v>
+        <v>Cheque</v>
       </c>
       <c r="P3" t="str">
         <v>DEALER</v>
@@ -538,25 +541,25 @@
         <v>Pahadiya Commercial Ltd</v>
       </c>
       <c r="C4" t="str">
-        <v>3005/405733793/00/000</v>
+        <v>3005/406819955/00/000</v>
       </c>
       <c r="D4" t="str">
-        <v>ME4JC85MFSD048920</v>
+        <v>ME4JF481GE8173192</v>
       </c>
       <c r="E4" t="str">
         <v>TWO WHEELER</v>
       </c>
       <c r="F4" t="str">
-        <v>New Business</v>
+        <v>Roll Over</v>
       </c>
       <c r="G4" t="str">
-        <v>2025-08-28T19:48:15.328022</v>
+        <v>2025-09-02T13:09:01.335899</v>
       </c>
       <c r="H4" t="str">
-        <v>Sneha Bharti</v>
+        <v>Punam Bhaskar</v>
       </c>
       <c r="I4" t="str">
-        <v>6051</v>
+        <v>1296</v>
       </c>
       <c r="J4" t="str">
         <v>12345678</v>
@@ -565,7 +568,7 @@
         <v>HONDA MOTORCYCLE</v>
       </c>
       <c r="N4" t="str">
-        <v>SHINE 125 DISC OBD2B</v>
+        <v>ACTIVA I</v>
       </c>
       <c r="O4" t="str">
         <v>Insta</v>
@@ -585,10 +588,10 @@
         <v>Pahadiya Commercial Ltd</v>
       </c>
       <c r="C5" t="str">
-        <v>3005/O/405511396/00/000</v>
+        <v>3005/405916108/00/000</v>
       </c>
       <c r="D5" t="str">
-        <v>ME4JK157DPW044682</v>
+        <v>ME4JF505JG8247812</v>
       </c>
       <c r="E5" t="str">
         <v>TWO WHEELER</v>
@@ -597,25 +600,25 @@
         <v>Roll Over</v>
       </c>
       <c r="G5" t="str">
-        <v>2025-08-27T14:21:59.8857</v>
+        <v>2025-08-29T16:33:16.847646</v>
       </c>
       <c r="H5" t="str">
-        <v>Anita Devi</v>
+        <v>Dinesh Prasad Singh</v>
       </c>
       <c r="I5" t="str">
-        <v>1735</v>
+        <v>2001</v>
       </c>
       <c r="J5" t="str">
-        <v>1245192604</v>
+        <v>1245389166</v>
       </c>
       <c r="K5" t="str">
-        <v>855854</v>
+        <v>855484</v>
       </c>
       <c r="M5" t="str">
         <v>HONDA MOTORCYCLE</v>
       </c>
       <c r="N5" t="str">
-        <v>ACTIVA 6G H SMART OBD2</v>
+        <v>ACTIVA 3G</v>
       </c>
       <c r="O5" t="str">
         <v>Cheque</v>
@@ -635,37 +638,37 @@
         <v>Pahadiya Commercial Ltd</v>
       </c>
       <c r="C6" t="str">
-        <v>3005/405552561/00/000</v>
+        <v>3005/406284332/00/000</v>
       </c>
       <c r="D6" t="str">
-        <v>ME4JC94FGSD015602</v>
+        <v>ME4JF49BGKW027827</v>
       </c>
       <c r="E6" t="str">
         <v>TWO WHEELER</v>
       </c>
       <c r="F6" t="str">
-        <v>New Business</v>
+        <v>Roll Over</v>
       </c>
       <c r="G6" t="str">
-        <v>2025-08-27T19:43:12.038826</v>
+        <v>2025-08-30T16:47:45.989551</v>
       </c>
       <c r="H6" t="str">
-        <v>SHASHANK SHEKHAR</v>
+        <v>Pawan Chowdhury</v>
       </c>
       <c r="I6" t="str">
-        <v>6236</v>
+        <v>1914</v>
       </c>
       <c r="J6" t="str">
-        <v>1245192604</v>
+        <v>1245479724</v>
       </c>
       <c r="K6" t="str">
-        <v>855854</v>
+        <v>744415</v>
       </c>
       <c r="M6" t="str">
         <v>HONDA MOTORCYCLE</v>
       </c>
       <c r="N6" t="str">
-        <v>NEW SP 125 DISC OBD2B</v>
+        <v>ACTIVA 125 ALLOY OBD2</v>
       </c>
       <c r="O6" t="str">
         <v>Cheque</v>
@@ -685,10 +688,10 @@
         <v>Pahadiya Commercial Ltd</v>
       </c>
       <c r="C7" t="str">
-        <v>3005/405677972/00/000</v>
+        <v>3005/406029796/00/000</v>
       </c>
       <c r="D7" t="str">
-        <v>ME4JK362FSW321998</v>
+        <v>ME4JK371HSW009517</v>
       </c>
       <c r="E7" t="str">
         <v>TWO WHEELER</v>
@@ -697,16 +700,19 @@
         <v>New Business</v>
       </c>
       <c r="G7" t="str">
-        <v>2025-08-28T15:09:43.851684</v>
+        <v>2025-08-29T20:48:32.473065</v>
       </c>
       <c r="H7" t="str">
-        <v>DrDayanand Singh</v>
+        <v>Rashid Ahmad</v>
       </c>
       <c r="I7" t="str">
-        <v>6188</v>
+        <v>6204</v>
       </c>
       <c r="J7" t="str">
-        <v>12345678</v>
+        <v>1245389166</v>
+      </c>
+      <c r="K7" t="str">
+        <v>855484</v>
       </c>
       <c r="M7" t="str">
         <v>HONDA MOTORCYCLE</v>
@@ -715,7 +721,7 @@
         <v>ACTIVA DLX OBD2B</v>
       </c>
       <c r="O7" t="str">
-        <v>Insta</v>
+        <v>Cheque</v>
       </c>
       <c r="P7" t="str">
         <v>DEALER</v>
@@ -732,10 +738,10 @@
         <v>Pahadiya Commercial Ltd</v>
       </c>
       <c r="C8" t="str">
-        <v>3005/405510382/00/000</v>
+        <v>3005/406615404/00/000</v>
       </c>
       <c r="D8" t="str">
-        <v>ME4JC94JHSG001953</v>
+        <v>ME4JK431DSW011880</v>
       </c>
       <c r="E8" t="str">
         <v>TWO WHEELER</v>
@@ -744,25 +750,25 @@
         <v>New Business</v>
       </c>
       <c r="G8" t="str">
-        <v>2025-08-27T14:06:02.625651</v>
+        <v>2025-08-31T17:58:44.041589</v>
       </c>
       <c r="H8" t="str">
-        <v>Murari Kumar Singh</v>
+        <v>DIBYA KUMARI</v>
       </c>
       <c r="I8" t="str">
-        <v>6253</v>
+        <v>6706</v>
       </c>
       <c r="J8" t="str">
-        <v>1245192604</v>
+        <v>1245534626</v>
       </c>
       <c r="K8" t="str">
-        <v>855854</v>
+        <v>566988</v>
       </c>
       <c r="M8" t="str">
         <v>HONDA MOTORCYCLE</v>
       </c>
       <c r="N8" t="str">
-        <v>SP 125 ANNIVERSARY EDITION</v>
+        <v>ACTIVA 125 SMART OBD2B</v>
       </c>
       <c r="O8" t="str">
         <v>Cheque</v>
@@ -782,37 +788,40 @@
         <v>Pahadiya Commercial Ltd</v>
       </c>
       <c r="C9" t="str">
-        <v>3005/405662487/00/000</v>
+        <v>3005/405938028/00/000</v>
       </c>
       <c r="D9" t="str">
-        <v>ME4JC36JJC7161590</v>
+        <v>ME4JK361FSD069955</v>
       </c>
       <c r="E9" t="str">
         <v>TWO WHEELER</v>
       </c>
       <c r="F9" t="str">
-        <v>Roll Over</v>
+        <v>New Business</v>
       </c>
       <c r="G9" t="str">
-        <v>2025-08-28T13:01:21.797962</v>
+        <v>2025-08-29T18:50:07.264475</v>
       </c>
       <c r="H9" t="str">
-        <v>NAWDIP SINGH</v>
+        <v>ABDUL VAHAV</v>
       </c>
       <c r="I9" t="str">
-        <v>2050</v>
+        <v>5377</v>
       </c>
       <c r="J9" t="str">
-        <v>12345678</v>
+        <v>1245389166</v>
+      </c>
+      <c r="K9" t="str">
+        <v>855484</v>
       </c>
       <c r="M9" t="str">
         <v>HONDA MOTORCYCLE</v>
       </c>
       <c r="N9" t="str">
-        <v>CB SHINE</v>
+        <v>ACTIVA 110 STD OBD2B</v>
       </c>
       <c r="O9" t="str">
-        <v>Insta</v>
+        <v>Cheque</v>
       </c>
       <c r="P9" t="str">
         <v>DEALER</v>
@@ -829,37 +838,37 @@
         <v>Pahadiya Commercial Ltd</v>
       </c>
       <c r="C10" t="str">
-        <v>3005/405535533/00/000</v>
+        <v>3005/405938204/00/000</v>
       </c>
       <c r="D10" t="str">
-        <v>ME4JF497DH8013220</v>
+        <v>ME4JK361FSD071698</v>
       </c>
       <c r="E10" t="str">
         <v>TWO WHEELER</v>
       </c>
       <c r="F10" t="str">
-        <v>Roll Over</v>
+        <v>New Business</v>
       </c>
       <c r="G10" t="str">
-        <v>2025-08-27T14:53:03.42802</v>
+        <v>2025-08-29T18:52:52.633531</v>
       </c>
       <c r="H10" t="str">
-        <v>Vijay Kumar</v>
+        <v>Ravi Ranjan Kumar</v>
       </c>
       <c r="I10" t="str">
-        <v>1433</v>
+        <v>6014</v>
       </c>
       <c r="J10" t="str">
-        <v>1245192604</v>
+        <v>1245389166</v>
       </c>
       <c r="K10" t="str">
-        <v>855854</v>
+        <v>855484</v>
       </c>
       <c r="M10" t="str">
         <v>HONDA MOTORCYCLE</v>
       </c>
       <c r="N10" t="str">
-        <v>ACTIVA 125 DRUM ALLOY</v>
+        <v>ACTIVA 110 STD OBD2B</v>
       </c>
       <c r="O10" t="str">
         <v>Cheque</v>
@@ -879,25 +888,25 @@
         <v>Pahadiya Commercial Ltd</v>
       </c>
       <c r="C11" t="str">
-        <v>3005/405670437/00/000</v>
+        <v>3005/406795786/00/000</v>
       </c>
       <c r="D11" t="str">
-        <v>ME4JC94JHSG005129</v>
+        <v>ME4JF48BJH8034942</v>
       </c>
       <c r="E11" t="str">
         <v>TWO WHEELER</v>
       </c>
       <c r="F11" t="str">
-        <v>New Business</v>
+        <v>Roll Over</v>
       </c>
       <c r="G11" t="str">
-        <v>2025-08-28T14:01:48.6588</v>
+        <v>2025-09-02T12:13:43.229876</v>
       </c>
       <c r="H11" t="str">
-        <v>Lali Rawat</v>
+        <v>Gladis Sah</v>
       </c>
       <c r="I11" t="str">
-        <v>9760</v>
+        <v>1812</v>
       </c>
       <c r="J11" t="str">
         <v>12345678</v>
@@ -906,7 +915,7 @@
         <v>HONDA MOTORCYCLE</v>
       </c>
       <c r="N11" t="str">
-        <v>SP 125 ANNIVERSARY EDITION</v>
+        <v>ACTIVA</v>
       </c>
       <c r="O11" t="str">
         <v>Insta</v>
@@ -926,40 +935,28 @@
         <v>Pahadiya Commercial Ltd</v>
       </c>
       <c r="C12" t="str">
-        <v>3005/405546605/00/000</v>
-      </c>
-      <c r="D12" t="str">
-        <v>ME4JC94CGSG140723</v>
+        <v>3005/357901211/01/000</v>
       </c>
       <c r="E12" t="str">
         <v>TWO WHEELER</v>
       </c>
       <c r="F12" t="str">
-        <v>New Business</v>
+        <v>Renewal</v>
       </c>
       <c r="G12" t="str">
-        <v>2025-08-27T17:46:10.067243</v>
+        <v>2025-08-29T16:48:53</v>
       </c>
       <c r="H12" t="str">
-        <v>Guddu Kumar</v>
+        <v>Dileep Kumar Roy</v>
       </c>
       <c r="I12" t="str">
-        <v>6103</v>
+        <v>1119</v>
       </c>
       <c r="J12" t="str">
-        <v>1245192604</v>
-      </c>
-      <c r="K12" t="str">
-        <v>855854</v>
-      </c>
-      <c r="M12" t="str">
-        <v>HONDA MOTORCYCLE</v>
-      </c>
-      <c r="N12" t="str">
-        <v>NEW SP 125 DRUM OBD2B</v>
+        <v>1245324717</v>
       </c>
       <c r="O12" t="str">
-        <v>Cheque</v>
+        <v>Razorpay</v>
       </c>
       <c r="P12" t="str">
         <v>DEALER</v>
@@ -976,37 +973,37 @@
         <v>Pahadiya Commercial Ltd</v>
       </c>
       <c r="C13" t="str">
-        <v>3005/O/405500436/00/000</v>
+        <v>3005/405936341/00/000</v>
       </c>
       <c r="D13" t="str">
-        <v>ME4HC152HPG079717</v>
+        <v>ME4JC94JHSG003796</v>
       </c>
       <c r="E13" t="str">
         <v>TWO WHEELER</v>
       </c>
       <c r="F13" t="str">
-        <v>Roll Over</v>
+        <v>New Business</v>
       </c>
       <c r="G13" t="str">
-        <v>2025-08-27T11:33:08.494281</v>
+        <v>2025-08-29T18:31:55.53528</v>
       </c>
       <c r="H13" t="str">
-        <v>Navin Kumar Verma</v>
+        <v>Mohammad Shakil</v>
       </c>
       <c r="I13" t="str">
-        <v>1226</v>
+        <v>6253</v>
       </c>
       <c r="J13" t="str">
-        <v>1245192604</v>
+        <v>1245389166</v>
       </c>
       <c r="K13" t="str">
-        <v>855854</v>
+        <v>855484</v>
       </c>
       <c r="M13" t="str">
         <v>HONDA MOTORCYCLE</v>
       </c>
       <c r="N13" t="str">
-        <v>SHINE 100 OBD2</v>
+        <v>SP 125 ANNIVERSARY EDITION</v>
       </c>
       <c r="O13" t="str">
         <v>Cheque</v>
@@ -1026,10 +1023,10 @@
         <v>Pahadiya Commercial Ltd</v>
       </c>
       <c r="C14" t="str">
-        <v>3005/405502761/00/000</v>
+        <v>3005/406215871/00/000</v>
       </c>
       <c r="D14" t="str">
-        <v>ME4JC94CHSD042856</v>
+        <v>ME4JC94CHSD042881</v>
       </c>
       <c r="E14" t="str">
         <v>TWO WHEELER</v>
@@ -1038,19 +1035,19 @@
         <v>New Business</v>
       </c>
       <c r="G14" t="str">
-        <v>2025-08-27T12:10:08.200078</v>
+        <v>2025-08-30T14:04:21.347787</v>
       </c>
       <c r="H14" t="str">
-        <v>Adarsh Singh</v>
+        <v>Karn Kumar</v>
       </c>
       <c r="I14" t="str">
-        <v>5411</v>
+        <v>6103</v>
       </c>
       <c r="J14" t="str">
-        <v>1245192604</v>
+        <v>1245479724</v>
       </c>
       <c r="K14" t="str">
-        <v>855854</v>
+        <v>744415</v>
       </c>
       <c r="M14" t="str">
         <v>HONDA MOTORCYCLE</v>
@@ -1068,9 +1065,1435 @@
         <v>NYSA-LITE</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C15" t="str">
+        <v>3005/406818289/00/000</v>
+      </c>
+      <c r="D15" t="str">
+        <v>ME4JF502HE7174806</v>
+      </c>
+      <c r="E15" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F15" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G15" t="str">
+        <v>2025-09-02T12:48:36.740397</v>
+      </c>
+      <c r="H15" t="str">
+        <v>Braj Kishore Gupta</v>
+      </c>
+      <c r="I15" t="str">
+        <v>1352</v>
+      </c>
+      <c r="J15" t="str">
+        <v>12345678</v>
+      </c>
+      <c r="M15" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N15" t="str">
+        <v>ACTIVA.</v>
+      </c>
+      <c r="O15" t="str">
+        <v>Insta</v>
+      </c>
+      <c r="P15" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q15" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C16" t="str">
+        <v>3005/406350819/00/000</v>
+      </c>
+      <c r="D16" t="str">
+        <v>ME4JH010HSD002304</v>
+      </c>
+      <c r="E16" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F16" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G16" t="str">
+        <v>2025-08-30T18:48:08.118309</v>
+      </c>
+      <c r="H16" t="str">
+        <v>VISHAL KUMAR</v>
+      </c>
+      <c r="I16" t="str">
+        <v>6411</v>
+      </c>
+      <c r="J16" t="str">
+        <v>1245479724</v>
+      </c>
+      <c r="K16" t="str">
+        <v>744415</v>
+      </c>
+      <c r="M16" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N16" t="str">
+        <v>CB125 HORNET OBD2B</v>
+      </c>
+      <c r="O16" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P16" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q16" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C17" t="str">
+        <v>3005/406783644/00/B00</v>
+      </c>
+      <c r="D17" t="str">
+        <v>ME4JC731DG8030515</v>
+      </c>
+      <c r="E17" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F17" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G17" t="str">
+        <v>2025-09-02T10:44:27</v>
+      </c>
+      <c r="H17" t="str">
+        <v>Ajeet Kumar</v>
+      </c>
+      <c r="I17" t="str">
+        <v>1180</v>
+      </c>
+      <c r="J17" t="str">
+        <v>1245619042</v>
+      </c>
+      <c r="M17" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N17" t="str">
+        <v>CB SHINE SP</v>
+      </c>
+      <c r="O17" t="str">
+        <v>Razorpay</v>
+      </c>
+      <c r="P17" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q17" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C18" t="str">
+        <v>3005/406579493/00/000</v>
+      </c>
+      <c r="D18" t="str">
+        <v>ME4JH010HSD003073</v>
+      </c>
+      <c r="E18" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F18" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G18" t="str">
+        <v>2025-08-31T15:13:27.574021</v>
+      </c>
+      <c r="H18" t="str">
+        <v>Rajiv Mistri</v>
+      </c>
+      <c r="I18" t="str">
+        <v>6411</v>
+      </c>
+      <c r="J18" t="str">
+        <v>1245534626</v>
+      </c>
+      <c r="K18" t="str">
+        <v>566988</v>
+      </c>
+      <c r="M18" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N18" t="str">
+        <v>CB 125 HORNET</v>
+      </c>
+      <c r="O18" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P18" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q18" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C19" t="str">
+        <v>3005/O/406417470/00/000</v>
+      </c>
+      <c r="D19" t="str">
+        <v>ME4JK155GPD026684</v>
+      </c>
+      <c r="E19" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F19" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G19" t="str">
+        <v>2025-08-30T19:35:44.541179</v>
+      </c>
+      <c r="H19" t="str">
+        <v>Arvind</v>
+      </c>
+      <c r="I19" t="str">
+        <v>1483</v>
+      </c>
+      <c r="J19" t="str">
+        <v>1245479724</v>
+      </c>
+      <c r="K19" t="str">
+        <v>744415</v>
+      </c>
+      <c r="M19" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N19" t="str">
+        <v>ACTIVA STD OBD2</v>
+      </c>
+      <c r="O19" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P19" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q19" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C20" t="str">
+        <v>3005/O/406203497/00/B00</v>
+      </c>
+      <c r="D20" t="str">
+        <v>ME4MC567DRA017145</v>
+      </c>
+      <c r="E20" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F20" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G20" t="str">
+        <v>2025-08-30T12:34:27.731059</v>
+      </c>
+      <c r="H20" t="str">
+        <v>Sonu Kumar</v>
+      </c>
+      <c r="I20" t="str">
+        <v>2754</v>
+      </c>
+      <c r="J20" t="str">
+        <v>1245479724</v>
+      </c>
+      <c r="K20" t="str">
+        <v>744415</v>
+      </c>
+      <c r="M20" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N20" t="str">
+        <v>HORNET 2.0</v>
+      </c>
+      <c r="O20" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P20" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q20" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C21" t="str">
+        <v>3005/406616414/00/000</v>
+      </c>
+      <c r="D21" t="str">
+        <v>ME4JC94EGSG313131</v>
+      </c>
+      <c r="E21" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F21" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G21" t="str">
+        <v>2025-08-31T18:12:35.091245</v>
+      </c>
+      <c r="H21" t="str">
+        <v>Suraj Keshari</v>
+      </c>
+      <c r="I21" t="str">
+        <v>9709</v>
+      </c>
+      <c r="J21" t="str">
+        <v>1245534626</v>
+      </c>
+      <c r="K21" t="str">
+        <v>566988</v>
+      </c>
+      <c r="M21" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N21" t="str">
+        <v>NEW SP 125 DISC OBD2B</v>
+      </c>
+      <c r="O21" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P21" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q21" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C22" t="str">
+        <v>3005/406755808/00/000</v>
+      </c>
+      <c r="D22" t="str">
+        <v>ME4JC831HLG063968</v>
+      </c>
+      <c r="E22" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F22" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G22" t="str">
+        <v>2025-09-01T17:46:05</v>
+      </c>
+      <c r="H22" t="str">
+        <v>Rajesh Kumar</v>
+      </c>
+      <c r="I22" t="str">
+        <v>2010</v>
+      </c>
+      <c r="J22" t="str">
+        <v>1245590673</v>
+      </c>
+      <c r="M22" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N22" t="str">
+        <v>SP 125 DISC BS VI</v>
+      </c>
+      <c r="O22" t="str">
+        <v>Razorpay</v>
+      </c>
+      <c r="P22" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q22" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C23" t="str">
+        <v>3005/405869045/00/000</v>
+      </c>
+      <c r="D23" t="str">
+        <v>ME4JF502HE8213082</v>
+      </c>
+      <c r="E23" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F23" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G23" t="str">
+        <v>2025-08-29T15:01:30.673508</v>
+      </c>
+      <c r="H23" t="str">
+        <v>Sandeep Kumar</v>
+      </c>
+      <c r="I23" t="str">
+        <v>1597</v>
+      </c>
+      <c r="J23" t="str">
+        <v>1245389166</v>
+      </c>
+      <c r="K23" t="str">
+        <v>855484</v>
+      </c>
+      <c r="M23" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N23" t="str">
+        <v>ACTIVA.</v>
+      </c>
+      <c r="O23" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P23" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q23" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C24" t="str">
+        <v>3005/406821293/00/000</v>
+      </c>
+      <c r="D24" t="str">
+        <v>ME4JK430FSW155592</v>
+      </c>
+      <c r="E24" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F24" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G24" t="str">
+        <v>2025-09-02T13:23:42.582354</v>
+      </c>
+      <c r="H24" t="str">
+        <v>Wasim Hussain</v>
+      </c>
+      <c r="I24" t="str">
+        <v>6280</v>
+      </c>
+      <c r="J24" t="str">
+        <v>12345678</v>
+      </c>
+      <c r="M24" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N24" t="str">
+        <v>ACTIVA 125 DISC OBD2B</v>
+      </c>
+      <c r="O24" t="str">
+        <v>Insta</v>
+      </c>
+      <c r="P24" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q24" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C25" t="str">
+        <v>3005/406208452/00/000</v>
+      </c>
+      <c r="D25" t="str">
+        <v>ME4JF49ABJU025968</v>
+      </c>
+      <c r="E25" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F25" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G25" t="str">
+        <v>2025-08-30T12:55:35.725516</v>
+      </c>
+      <c r="H25" t="str">
+        <v>Sanjay Kumar</v>
+      </c>
+      <c r="I25" t="str">
+        <v>4171</v>
+      </c>
+      <c r="J25" t="str">
+        <v>1245479724</v>
+      </c>
+      <c r="K25" t="str">
+        <v>744415</v>
+      </c>
+      <c r="M25" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N25" t="str">
+        <v>GRAZIA STD</v>
+      </c>
+      <c r="O25" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P25" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q25" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C26" t="str">
+        <v>3005/O/406291372/00/B00</v>
+      </c>
+      <c r="D26" t="str">
+        <v>ME4JF98HJPW003104</v>
+      </c>
+      <c r="E26" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F26" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G26" t="str">
+        <v>2025-08-30T17:27:12.688478</v>
+      </c>
+      <c r="H26" t="str">
+        <v>Geeta Devi</v>
+      </c>
+      <c r="I26" t="str">
+        <v>1462</v>
+      </c>
+      <c r="J26" t="str">
+        <v>1245479724</v>
+      </c>
+      <c r="K26" t="str">
+        <v>744415</v>
+      </c>
+      <c r="M26" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N26" t="str">
+        <v>DIO STD OBD2</v>
+      </c>
+      <c r="O26" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P26" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q26" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C27" t="str">
+        <v>3005/406711082/00/000</v>
+      </c>
+      <c r="D27" t="str">
+        <v>ME4JC73AHKD012383</v>
+      </c>
+      <c r="E27" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F27" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G27" t="str">
+        <v>2025-09-01T12:02:58.994412</v>
+      </c>
+      <c r="H27" t="str">
+        <v>RAMA KANT SINHA</v>
+      </c>
+      <c r="I27" t="str">
+        <v>1364</v>
+      </c>
+      <c r="J27" t="str">
+        <v>1245626111</v>
+      </c>
+      <c r="K27" t="str">
+        <v>658874</v>
+      </c>
+      <c r="M27" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N27" t="str">
+        <v>CB SHINE SP CBS</v>
+      </c>
+      <c r="O27" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P27" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q27" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C28" t="str">
+        <v>3005/405919465/00/000</v>
+      </c>
+      <c r="D28" t="str">
+        <v>ME4JC85NGSD106435</v>
+      </c>
+      <c r="E28" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F28" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G28" t="str">
+        <v>2025-08-29T16:37:22.310616</v>
+      </c>
+      <c r="H28" t="str">
+        <v>Amar Nath Mehta</v>
+      </c>
+      <c r="I28" t="str">
+        <v>9018</v>
+      </c>
+      <c r="J28" t="str">
+        <v>1245389166</v>
+      </c>
+      <c r="K28" t="str">
+        <v>855484</v>
+      </c>
+      <c r="M28" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N28" t="str">
+        <v>SHINE 125 DRUM OBD2B</v>
+      </c>
+      <c r="O28" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P28" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q28" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C29" t="str">
+        <v>3005/406293756/00/000</v>
+      </c>
+      <c r="D29" t="str">
+        <v>ME4JK361GSG094541</v>
+      </c>
+      <c r="E29" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F29" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G29" t="str">
+        <v>2025-08-30T17:49:48.17294</v>
+      </c>
+      <c r="H29" t="str">
+        <v>Binod Kumar</v>
+      </c>
+      <c r="I29" t="str">
+        <v>5377</v>
+      </c>
+      <c r="J29" t="str">
+        <v>1245479724</v>
+      </c>
+      <c r="K29" t="str">
+        <v>744415</v>
+      </c>
+      <c r="M29" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N29" t="str">
+        <v>ACTIVA 110 STD OBD2B</v>
+      </c>
+      <c r="O29" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P29" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q29" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C30" t="str">
+        <v>3005/406589554/00/000</v>
+      </c>
+      <c r="D30" t="str">
+        <v>ME4JC94EGSD076005</v>
+      </c>
+      <c r="E30" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F30" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G30" t="str">
+        <v>2025-08-31T17:08:37.032374</v>
+      </c>
+      <c r="H30" t="str">
+        <v>Sunil Kumar</v>
+      </c>
+      <c r="I30" t="str">
+        <v>9709</v>
+      </c>
+      <c r="J30" t="str">
+        <v>1245534626</v>
+      </c>
+      <c r="K30" t="str">
+        <v>566988</v>
+      </c>
+      <c r="M30" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N30" t="str">
+        <v>NEW SP 125 DISC OBD2B</v>
+      </c>
+      <c r="O30" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P30" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q30" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C31" t="str">
+        <v>3005/O/405865842/00/000</v>
+      </c>
+      <c r="D31" t="str">
+        <v>ME4JC856GMD209409</v>
+      </c>
+      <c r="E31" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F31" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G31" t="str">
+        <v>2025-08-29T14:50:00.599992</v>
+      </c>
+      <c r="H31" t="str">
+        <v>Rakesh Kumar</v>
+      </c>
+      <c r="I31" t="str">
+        <v>1320</v>
+      </c>
+      <c r="J31" t="str">
+        <v>1245389166</v>
+      </c>
+      <c r="K31" t="str">
+        <v>855484</v>
+      </c>
+      <c r="M31" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N31" t="str">
+        <v>CB SHINE DRUM BS VI</v>
+      </c>
+      <c r="O31" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P31" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q31" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C32" t="str">
+        <v>3005/406739497/00/B00</v>
+      </c>
+      <c r="D32" t="str">
+        <v>ME4JF50BCK7163894</v>
+      </c>
+      <c r="E32" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F32" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G32" t="str">
+        <v>2025-09-01T14:30:31</v>
+      </c>
+      <c r="H32" t="str">
+        <v>Ravindra Vishwakarma</v>
+      </c>
+      <c r="I32" t="str">
+        <v>4624</v>
+      </c>
+      <c r="J32" t="str">
+        <v>1245569067</v>
+      </c>
+      <c r="M32" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N32" t="str">
+        <v>ACTIVA 5G DLX</v>
+      </c>
+      <c r="O32" t="str">
+        <v>Razorpay</v>
+      </c>
+      <c r="P32" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q32" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C33" t="str">
+        <v>3005/406578994/00/000</v>
+      </c>
+      <c r="D33" t="str">
+        <v>ME4JC94CGSG142045</v>
+      </c>
+      <c r="E33" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F33" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G33" t="str">
+        <v>2025-08-31T15:04:57.564868</v>
+      </c>
+      <c r="H33" t="str">
+        <v>Bittu Raj</v>
+      </c>
+      <c r="I33" t="str">
+        <v>6103</v>
+      </c>
+      <c r="J33" t="str">
+        <v>1245534626</v>
+      </c>
+      <c r="K33" t="str">
+        <v>566988</v>
+      </c>
+      <c r="M33" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N33" t="str">
+        <v>NEW SP 125 DRUM OBD2B</v>
+      </c>
+      <c r="O33" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P33" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q33" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C34" t="str">
+        <v>3005/406788582/00/000</v>
+      </c>
+      <c r="D34" t="str">
+        <v>ME4JF49NHLD009958</v>
+      </c>
+      <c r="E34" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F34" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G34" t="str">
+        <v>2025-09-02T11:17:19.722981</v>
+      </c>
+      <c r="H34" t="str">
+        <v>JYOTI KUMARI</v>
+      </c>
+      <c r="I34" t="str">
+        <v>1353</v>
+      </c>
+      <c r="J34" t="str">
+        <v>12345678</v>
+      </c>
+      <c r="M34" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N34" t="str">
+        <v>ACTIVA 125 DRUM ALLOY</v>
+      </c>
+      <c r="O34" t="str">
+        <v>Insta</v>
+      </c>
+      <c r="P34" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q34" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C35" t="str">
+        <v>3005/406626986/00/000</v>
+      </c>
+      <c r="D35" t="str">
+        <v>ME4JK362GSW339191</v>
+      </c>
+      <c r="E35" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F35" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G35" t="str">
+        <v>2025-08-31T19:41:19.597979</v>
+      </c>
+      <c r="H35" t="str">
+        <v>Amarendra Kumar</v>
+      </c>
+      <c r="I35" t="str">
+        <v>9775</v>
+      </c>
+      <c r="J35" t="str">
+        <v>1245534626</v>
+      </c>
+      <c r="K35" t="str">
+        <v>566988</v>
+      </c>
+      <c r="M35" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N35" t="str">
+        <v>ACTIVA DLX OBD2B</v>
+      </c>
+      <c r="O35" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P35" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q35" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C36" t="str">
+        <v>3005/406720974/00/000</v>
+      </c>
+      <c r="D36" t="str">
+        <v>ME4JK431DSW012810</v>
+      </c>
+      <c r="E36" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F36" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G36" t="str">
+        <v>2025-09-01T12:36:18.283465</v>
+      </c>
+      <c r="H36" t="str">
+        <v>ANIL KUMAR</v>
+      </c>
+      <c r="I36" t="str">
+        <v>10283</v>
+      </c>
+      <c r="J36" t="str">
+        <v>1245626111</v>
+      </c>
+      <c r="K36" t="str">
+        <v>658874</v>
+      </c>
+      <c r="M36" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N36" t="str">
+        <v>ACTIVA 125 SMART OBD2B</v>
+      </c>
+      <c r="O36" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P36" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q36" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C37" t="str">
+        <v>3005/406588547/00/000</v>
+      </c>
+      <c r="D37" t="str">
+        <v>ME4JK430GSG110948</v>
+      </c>
+      <c r="E37" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F37" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G37" t="str">
+        <v>2025-08-31T16:49:21.247581</v>
+      </c>
+      <c r="H37" t="str">
+        <v>Ashutosh Raj</v>
+      </c>
+      <c r="I37" t="str">
+        <v>6280</v>
+      </c>
+      <c r="J37" t="str">
+        <v>1245534626</v>
+      </c>
+      <c r="K37" t="str">
+        <v>566988</v>
+      </c>
+      <c r="M37" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N37" t="str">
+        <v>ACTIVA 125 DISC OBD2B</v>
+      </c>
+      <c r="O37" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P37" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q37" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C38" t="str">
+        <v>3005/406743492/00/000</v>
+      </c>
+      <c r="D38" t="str">
+        <v>ME4JK361FSD071374</v>
+      </c>
+      <c r="E38" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F38" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G38" t="str">
+        <v>2025-09-01T15:28:42.514605</v>
+      </c>
+      <c r="H38" t="str">
+        <v>Karan Kumar</v>
+      </c>
+      <c r="I38" t="str">
+        <v>6014</v>
+      </c>
+      <c r="J38" t="str">
+        <v>1245626111</v>
+      </c>
+      <c r="K38" t="str">
+        <v>658874</v>
+      </c>
+      <c r="M38" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N38" t="str">
+        <v>ACTIVA 110 STD OBD2B</v>
+      </c>
+      <c r="O38" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P38" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q38" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C39" t="str">
+        <v>3005/406826756/00/000</v>
+      </c>
+      <c r="D39" t="str">
+        <v>ME4JC654GH7154044</v>
+      </c>
+      <c r="E39" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F39" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G39" t="str">
+        <v>2025-09-02T14:31:00.295423</v>
+      </c>
+      <c r="H39" t="str">
+        <v>Ravi Kumar</v>
+      </c>
+      <c r="I39" t="str">
+        <v>2039</v>
+      </c>
+      <c r="J39" t="str">
+        <v>12345678</v>
+      </c>
+      <c r="M39" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N39" t="str">
+        <v>CB SHINE</v>
+      </c>
+      <c r="O39" t="str">
+        <v>Insta</v>
+      </c>
+      <c r="P39" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q39" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C40" t="str">
+        <v>3005/405820461/00/000</v>
+      </c>
+      <c r="D40" t="str">
+        <v>ME4JC85NGSD106401</v>
+      </c>
+      <c r="E40" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F40" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G40" t="str">
+        <v>2025-08-29T12:32:35.743281</v>
+      </c>
+      <c r="H40" t="str">
+        <v>Chandan Kumar</v>
+      </c>
+      <c r="I40" t="str">
+        <v>5974</v>
+      </c>
+      <c r="J40" t="str">
+        <v>1245389166</v>
+      </c>
+      <c r="K40" t="str">
+        <v>855484</v>
+      </c>
+      <c r="M40" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N40" t="str">
+        <v>SHINE 125 DRUM OBD2B</v>
+      </c>
+      <c r="O40" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P40" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q40" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C41" t="str">
+        <v>3005/405872828/00/000</v>
+      </c>
+      <c r="D41" t="str">
+        <v>ME4JC94JHSG005112</v>
+      </c>
+      <c r="E41" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F41" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G41" t="str">
+        <v>2025-08-29T15:17:54.194918</v>
+      </c>
+      <c r="H41" t="str">
+        <v>Vinay Kumar</v>
+      </c>
+      <c r="I41" t="str">
+        <v>6253</v>
+      </c>
+      <c r="J41" t="str">
+        <v>1245389166</v>
+      </c>
+      <c r="K41" t="str">
+        <v>855484</v>
+      </c>
+      <c r="M41" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N41" t="str">
+        <v>SP 125 ANNIVERSARY EDITION</v>
+      </c>
+      <c r="O41" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P41" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q41" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C42" t="str">
+        <v>3005/405934226/00/000</v>
+      </c>
+      <c r="D42" t="str">
+        <v>ME4JC85NGSD105971</v>
+      </c>
+      <c r="E42" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F42" t="str">
+        <v>New Business</v>
+      </c>
+      <c r="G42" t="str">
+        <v>2025-08-29T18:10:16.818705</v>
+      </c>
+      <c r="H42" t="str">
+        <v>Chhathu Kumar</v>
+      </c>
+      <c r="I42" t="str">
+        <v>5974</v>
+      </c>
+      <c r="J42" t="str">
+        <v>1245389166</v>
+      </c>
+      <c r="K42" t="str">
+        <v>855484</v>
+      </c>
+      <c r="M42" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N42" t="str">
+        <v>SHINE 125 DRUM OBD2B</v>
+      </c>
+      <c r="O42" t="str">
+        <v>Cheque</v>
+      </c>
+      <c r="P42" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q42" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>IM-568754</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Pahadiya Commercial Ltd</v>
+      </c>
+      <c r="C43" t="str">
+        <v>3005/O/406825906/00/000</v>
+      </c>
+      <c r="D43" t="str">
+        <v>ME4JK158GRG000780</v>
+      </c>
+      <c r="E43" t="str">
+        <v>TWO WHEELER</v>
+      </c>
+      <c r="F43" t="str">
+        <v>Roll Over</v>
+      </c>
+      <c r="G43" t="str">
+        <v>2025-09-02T14:18:50.525919</v>
+      </c>
+      <c r="H43" t="str">
+        <v>PANKAJ  JAIN</v>
+      </c>
+      <c r="I43" t="str">
+        <v>1653</v>
+      </c>
+      <c r="J43" t="str">
+        <v>12345678</v>
+      </c>
+      <c r="M43" t="str">
+        <v>HONDA MOTORCYCLE</v>
+      </c>
+      <c r="N43" t="str">
+        <v>ACTIVA DLX OBD2</v>
+      </c>
+      <c r="O43" t="str">
+        <v>Insta</v>
+      </c>
+      <c r="P43" t="str">
+        <v>DEALER</v>
+      </c>
+      <c r="Q43" t="str">
+        <v>NYSA-LITE</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q43"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>